<commit_message>
updates in  topic 4
</commit_message>
<xml_diff>
--- a/topic_4_img/Topic 4 Sol.xlsx
+++ b/topic_4_img/Topic 4 Sol.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t xml:space="preserve">Part 1</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t xml:space="preserve">R: the net income will increase by almost 3k euros that year relative to the base scenario. The company must inform in the 2013 report about the accounting change. No need to restate the 2012 report.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.bayer.com/en/investors/integrated-annual-reportshttps://www.bayer.com/en/investors/integrated-annual-reports</t>
   </si>
   <si>
     <t xml:space="preserve">For clarity, I will paste here the tables from the PDF, but students can just write down the numbers needed.</t>
@@ -269,6 +266,7 @@
       <color rgb="FF0000EE"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -517,9 +515,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>730440</xdr:colOff>
+      <xdr:colOff>730080</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>100080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -529,7 +527,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="394200" y="24480"/>
-          <a:ext cx="8741880" cy="2180880"/>
+          <a:ext cx="8741520" cy="2180520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -560,6 +558,7 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -567,21 +566,23 @@
             <a:t>At the end of the annual accounting period, December 31, 2012, O’Connor Company’s records reflected the following for information for one on its machines: </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -589,21 +590,23 @@
             <a:t>- Cost when acquired $30,000 </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -611,32 +614,35 @@
             <a:t>- Accumulated depreciation $10,200</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -644,32 +650,35 @@
             <a:t>During January 2013, the machine was renovated at a cost of $15,500 paid in cash. As a result, the estimated useful life increased from five years (original estimation) to eight years (updated estimation in Jan 2013), and the residual value increased from $4,500 to $6,500. The company uses straight-line depreciation. </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -677,21 +686,23 @@
             <a:t>Required: </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -699,21 +710,23 @@
             <a:t>1. How did the renovation impact the balance sheet in January 2013? did it also impacted the income statement?</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -721,21 +734,23 @@
             <a:t>2. How old was the machine at the end of 2012? </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -743,21 +758,23 @@
             <a:t>3. How much is the new straight-line depreciation expense for the year 2013? </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -765,17 +782,19 @@
             <a:t>4. Analyze how your response in 3 would change if a software update of the Machine drives the extension in the estimated life and residual value without needing any renovation expense. What would be the effect on net income? What are the reporting requirements for this update on estimates?</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+            <a:effectLst/>
             <a:uFillTx/>
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
@@ -798,9 +817,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>3215160</xdr:colOff>
+      <xdr:colOff>3214800</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>73080</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -810,7 +829,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="476280" y="97560"/>
-          <a:ext cx="10500480" cy="1622160"/>
+          <a:ext cx="10500120" cy="1621800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -841,6 +860,7 @@
               <a:solidFill>
                 <a:srgbClr val="0000ee"/>
               </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -853,6 +873,7 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -860,32 +881,35 @@
             <a:t> → Annual Report 2012</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -893,21 +917,23 @@
             <a:t>1) Income Statement: How much was the income before taxes  in 2012?</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -915,21 +941,23 @@
             <a:t>2) Notes 10 and 11:</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -941,6 +969,7 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -948,21 +977,23 @@
             <a:t>2.1: Is "other operating income" a relevant component of net income? </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -974,6 +1005,7 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -981,21 +1013,23 @@
             <a:t>2.2: What events generated “miscelaneous operating income”? </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -1007,6 +1041,7 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -1018,6 +1053,7 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -1025,21 +1061,23 @@
             <a:t>	</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -1051,6 +1089,7 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -1058,21 +1097,23 @@
             <a:t>2.4: What fraction of the “other operating expenses” is driven by special items? How much of them are not being explained?</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -1084,6 +1125,7 @@
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -1091,32 +1133,35 @@
             <a:t>2.5: What events generated “other operating expenses: Miscellaneuous”? Are they recurring expenses?</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
               <a:uFillTx/>
               <a:latin typeface="Times New Roman"/>
               <a:ea typeface="DejaVu Sans"/>
@@ -1124,17 +1169,19 @@
             <a:t>Response: </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
-            <a:uFillTx/>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" strike="noStrike" u="none">
+            <a:effectLst/>
             <a:uFillTx/>
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
@@ -1259,11 +1306,11 @@
   </sheetPr>
   <dimension ref="A19:E46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C42" activeCellId="1" sqref="J33:J34 C42"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E48" activeCellId="0" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.71"/>
   </cols>
@@ -1459,11 +1506,11 @@
   </sheetPr>
   <dimension ref="B1:K58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J34" activeCellId="0" sqref="J33:J34"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="7" width="11.57"/>
@@ -1471,26 +1518,24 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="7" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="8" t="s">
-        <v>22</v>
-      </c>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -1517,7 +1562,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="7" t="n">
         <v>195</v>
@@ -1526,7 +1571,7 @@
         <v>226</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I19" s="7" t="n">
         <v>18</v>
@@ -1537,7 +1582,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="7" t="n">
         <v>42</v>
@@ -1546,7 +1591,7 @@
         <v>28</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I20" s="7" t="n">
         <v>4</v>
@@ -1557,7 +1602,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="7" t="n">
         <v>50</v>
@@ -1566,7 +1611,7 @@
         <v>69</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I21" s="7" t="n">
         <v>13</v>
@@ -1577,7 +1622,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="7" t="n">
         <v>138</v>
@@ -1586,18 +1631,18 @@
         <v>171</v>
       </c>
       <c r="H22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="J22" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="7" t="n">
         <v>434</v>
@@ -1606,7 +1651,7 @@
         <v>589</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I23" s="11" t="n">
         <v>136</v>
@@ -1617,7 +1662,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D24" s="13" t="n">
         <v>859</v>
@@ -1626,7 +1671,7 @@
         <v>1083</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I24" s="14" t="n">
         <v>171</v>
@@ -1637,7 +1682,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" s="7" t="n">
         <v>171</v>
@@ -1648,14 +1693,14 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
@@ -1680,15 +1725,15 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I29" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" s="7" t="n">
         <v>-20</v>
@@ -1697,7 +1742,7 @@
         <v>-26</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I30" s="7" t="n">
         <v>-150</v>
@@ -1708,7 +1753,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D31" s="7" t="n">
         <v>-62</v>
@@ -1717,7 +1762,7 @@
         <v>-95</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I31" s="7" t="n">
         <v>-139</v>
@@ -1728,7 +1773,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D32" s="7" t="n">
         <v>-260</v>
@@ -1737,7 +1782,7 @@
         <v>-1298</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I32" s="7" t="n">
         <v>-64</v>
@@ -1748,7 +1793,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D33" s="7" t="n">
         <v>-130</v>
@@ -1757,7 +1802,7 @@
         <v>-324</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I33" s="7" t="n">
         <v>-443</v>
@@ -1768,7 +1813,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D34" s="15" t="n">
         <v>-1188</v>
@@ -1777,7 +1822,7 @@
         <v>-1215</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I34" s="17" t="n">
         <v>-1026</v>
@@ -1788,7 +1833,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" s="17" t="n">
         <v>-1660</v>
@@ -1799,7 +1844,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D37" s="15" t="n">
         <v>-1026</v>
@@ -1810,10 +1855,10 @@
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D41" s="19" t="n">
         <v>3248</v>
@@ -1821,10 +1866,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D44" s="20" t="n">
         <f aca="false">E24/D41</f>
@@ -1833,23 +1878,23 @@
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D49" s="20" t="n">
         <f aca="false">J23/J24</f>
@@ -1858,15 +1903,15 @@
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="D52" s="20" t="n">
         <f aca="false">E37/E35</f>
@@ -1875,12 +1920,12 @@
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D54" s="20" t="n">
         <f aca="false">J33/J34</f>
@@ -1889,20 +1934,20 @@
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>